<commit_message>
updated resources, added problem statement latex file
</commit_message>
<xml_diff>
--- a/ADSDataPoints_comments.xlsx
+++ b/ADSDataPoints_comments.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2057" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="695">
   <si>
     <t xml:space="preserve">Info:
 AT %Q* stands for outgoing values from PLC perspective
@@ -682,6 +682,9 @@
     <t xml:space="preserve">fAHUFlapETAActADS </t>
   </si>
   <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">fAHUFlapETASetADS </t>
   </si>
   <si>
@@ -793,49 +796,13 @@
     <t xml:space="preserve">fAHUPHValveActADS</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">// </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Actual valve opening</t>
-    </r>
+    <t xml:space="preserve">// Actual valve opening</t>
   </si>
   <si>
     <t xml:space="preserve">fAHUPHValveSetADS</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">// </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Setpoint for valve opening</t>
-    </r>
+    <t xml:space="preserve">// Setpoint for valve opening</t>
   </si>
   <si>
     <t xml:space="preserve">fAHUPHValveSetADSmirror</t>
@@ -2150,7 +2117,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2172,12 +2139,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2260,8 +2221,8 @@
   </sheetPr>
   <dimension ref="A1:E761"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A242" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E264" activeCellId="0" sqref="E264"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A316" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A333" activeCellId="0" sqref="A333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4571,10 +4532,13 @@
       <c r="C231" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="D231" s="0" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B232" s="0" t="s">
         <v>23</v>
@@ -4585,7 +4549,7 @@
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B233" s="0" t="s">
         <v>3</v>
@@ -4596,7 +4560,7 @@
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B234" s="0" t="s">
         <v>3</v>
@@ -4607,7 +4571,7 @@
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B235" s="0" t="s">
         <v>23</v>
@@ -4618,7 +4582,7 @@
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B236" s="0" t="s">
         <v>3</v>
@@ -4629,7 +4593,7 @@
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B237" s="0" t="s">
         <v>3</v>
@@ -4640,7 +4604,7 @@
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B238" s="0" t="s">
         <v>23</v>
@@ -4651,7 +4615,7 @@
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B239" s="0" t="s">
         <v>3</v>
@@ -4662,12 +4626,12 @@
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B241" s="0" t="s">
         <v>3</v>
@@ -4678,7 +4642,7 @@
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B242" s="0" t="s">
         <v>23</v>
@@ -4689,7 +4653,7 @@
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B243" s="0" t="s">
         <v>3</v>
@@ -4700,7 +4664,7 @@
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B244" s="0" t="s">
         <v>3</v>
@@ -4711,7 +4675,7 @@
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B245" s="0" t="s">
         <v>3</v>
@@ -4722,7 +4686,7 @@
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B246" s="0" t="s">
         <v>3</v>
@@ -4733,7 +4697,7 @@
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B247" s="0" t="s">
         <v>23</v>
@@ -4744,7 +4708,7 @@
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B248" s="0" t="s">
         <v>3</v>
@@ -4755,7 +4719,7 @@
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B249" s="0" t="s">
         <v>3</v>
@@ -4766,7 +4730,7 @@
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B250" s="0" t="s">
         <v>3</v>
@@ -4782,7 +4746,7 @@
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B252" s="0" t="s">
         <v>3</v>
@@ -4793,7 +4757,7 @@
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B253" s="0" t="s">
         <v>3</v>
@@ -4804,7 +4768,7 @@
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B254" s="0" t="s">
         <v>3</v>
@@ -4815,7 +4779,7 @@
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B255" s="0" t="s">
         <v>3</v>
@@ -4826,7 +4790,7 @@
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B256" s="0" t="s">
         <v>3</v>
@@ -4837,12 +4801,12 @@
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B258" s="0" t="s">
         <v>3</v>
@@ -4853,7 +4817,7 @@
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B259" s="0" t="s">
         <v>3</v>
@@ -4864,7 +4828,7 @@
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B260" s="0" t="s">
         <v>3</v>
@@ -4875,7 +4839,7 @@
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B261" s="0" t="s">
         <v>3</v>
@@ -4886,12 +4850,12 @@
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B263" s="0" t="s">
         <v>3</v>
@@ -4899,10 +4863,13 @@
       <c r="C263" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="D263" s="0" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4912,7 +4879,7 @@
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B266" s="0" t="s">
         <v>3</v>
@@ -4923,7 +4890,7 @@
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B267" s="0" t="s">
         <v>3</v>
@@ -4934,7 +4901,7 @@
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B268" s="0" t="s">
         <v>3</v>
@@ -4945,7 +4912,7 @@
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B269" s="0" t="s">
         <v>3</v>
@@ -4961,7 +4928,7 @@
     </row>
     <row r="271" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B271" s="0" t="s">
         <v>3</v>
@@ -4969,13 +4936,16 @@
       <c r="C271" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="D271" s="0" t="s">
+        <v>219</v>
+      </c>
       <c r="E271" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B272" s="0" t="s">
         <v>23</v>
@@ -4983,13 +4953,16 @@
       <c r="C272" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="D272" s="0" t="s">
+        <v>219</v>
+      </c>
       <c r="E272" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B273" s="0" t="s">
         <v>3</v>
@@ -5005,7 +4978,7 @@
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B275" s="0" t="s">
         <v>23</v>
@@ -5013,10 +4986,13 @@
       <c r="C275" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="D275" s="0" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B276" s="0" t="s">
         <v>3</v>
@@ -5027,7 +5003,7 @@
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B277" s="0" t="s">
         <v>3</v>
@@ -5038,7 +5014,7 @@
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B278" s="0" t="s">
         <v>3</v>
@@ -5049,7 +5025,7 @@
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B279" s="0" t="s">
         <v>3</v>
@@ -5060,7 +5036,7 @@
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B280" s="0" t="s">
         <v>3</v>
@@ -5071,7 +5047,7 @@
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B281" s="0" t="s">
         <v>3</v>
@@ -5082,7 +5058,7 @@
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B282" s="0" t="s">
         <v>23</v>
@@ -5093,7 +5069,7 @@
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B283" s="0" t="s">
         <v>3</v>
@@ -5104,7 +5080,7 @@
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B284" s="0" t="s">
         <v>3</v>
@@ -5115,7 +5091,7 @@
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B285" s="0" t="s">
         <v>3</v>
@@ -5126,12 +5102,12 @@
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B287" s="0" t="s">
         <v>3</v>
@@ -5142,7 +5118,7 @@
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B288" s="0" t="s">
         <v>3</v>
@@ -5153,7 +5129,7 @@
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B289" s="0" t="s">
         <v>23</v>
@@ -5164,7 +5140,7 @@
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B290" s="0" t="s">
         <v>3</v>
@@ -5175,7 +5151,7 @@
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B291" s="0" t="s">
         <v>3</v>
@@ -5186,7 +5162,7 @@
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5196,7 +5172,7 @@
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B294" s="0" t="s">
         <v>3</v>
@@ -5207,7 +5183,7 @@
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B295" s="0" t="s">
         <v>3</v>
@@ -5218,7 +5194,7 @@
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B296" s="0" t="s">
         <v>3</v>
@@ -5229,7 +5205,7 @@
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B297" s="0" t="s">
         <v>3</v>
@@ -5240,10 +5216,10 @@
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B298" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C298" s="0" t="s">
         <v>19</v>
@@ -5251,10 +5227,10 @@
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B299" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C299" s="0" t="s">
         <v>19</v>
@@ -5262,7 +5238,7 @@
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B300" s="0" t="s">
         <v>3</v>
@@ -5278,7 +5254,7 @@
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B302" s="0" t="s">
         <v>3</v>
@@ -5289,7 +5265,7 @@
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B303" s="0" t="s">
         <v>23</v>
@@ -5300,7 +5276,7 @@
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B304" s="0" t="s">
         <v>3</v>
@@ -5316,7 +5292,7 @@
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B306" s="0" t="s">
         <v>23</v>
@@ -5327,7 +5303,7 @@
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B307" s="0" t="s">
         <v>3</v>
@@ -5338,7 +5314,7 @@
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B308" s="0" t="s">
         <v>3</v>
@@ -5349,7 +5325,7 @@
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B309" s="0" t="s">
         <v>3</v>
@@ -5360,7 +5336,7 @@
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B310" s="0" t="s">
         <v>3</v>
@@ -5371,7 +5347,7 @@
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B311" s="0" t="s">
         <v>3</v>
@@ -5382,7 +5358,7 @@
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B312" s="0" t="s">
         <v>3</v>
@@ -5390,10 +5366,13 @@
       <c r="C312" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="D312" s="0" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B313" s="0" t="s">
         <v>23</v>
@@ -5404,7 +5383,7 @@
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B314" s="0" t="s">
         <v>3</v>
@@ -5415,7 +5394,7 @@
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B315" s="0" t="s">
         <v>3</v>
@@ -5426,18 +5405,21 @@
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B316" s="0" t="s">
         <v>3</v>
       </c>
       <c r="C316" s="0" t="s">
         <v>19</v>
+      </c>
+      <c r="D316" s="0" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5447,7 +5429,7 @@
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B319" s="0" t="s">
         <v>3</v>
@@ -5458,7 +5440,7 @@
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B320" s="0" t="s">
         <v>3</v>
@@ -5469,7 +5451,7 @@
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B321" s="0" t="s">
         <v>3</v>
@@ -5480,7 +5462,7 @@
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B322" s="0" t="s">
         <v>3</v>
@@ -5496,7 +5478,7 @@
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B324" s="0" t="s">
         <v>3</v>
@@ -5507,7 +5489,7 @@
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B325" s="0" t="s">
         <v>23</v>
@@ -5518,7 +5500,7 @@
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B326" s="0" t="s">
         <v>3</v>
@@ -5534,7 +5516,7 @@
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B328" s="0" t="s">
         <v>23</v>
@@ -5545,7 +5527,7 @@
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B329" s="0" t="s">
         <v>3</v>
@@ -5556,7 +5538,7 @@
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B330" s="0" t="s">
         <v>3</v>
@@ -5567,7 +5549,7 @@
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B331" s="0" t="s">
         <v>3</v>
@@ -5578,7 +5560,7 @@
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B332" s="0" t="s">
         <v>3</v>
@@ -5589,7 +5571,7 @@
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B333" s="0" t="s">
         <v>3</v>
@@ -5600,7 +5582,7 @@
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B334" s="0" t="s">
         <v>3</v>
@@ -5611,7 +5593,7 @@
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B335" s="0" t="s">
         <v>23</v>
@@ -5622,7 +5604,7 @@
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B336" s="0" t="s">
         <v>3</v>
@@ -5633,7 +5615,7 @@
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B337" s="0" t="s">
         <v>3</v>
@@ -5644,7 +5626,7 @@
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B338" s="0" t="s">
         <v>3</v>
@@ -5655,12 +5637,12 @@
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B340" s="0" t="s">
         <v>23</v>
@@ -5668,10 +5650,13 @@
       <c r="C340" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="D340" s="0" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B341" s="0" t="s">
         <v>3</v>
@@ -5682,17 +5667,17 @@
     </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B345" s="0" t="s">
         <v>23</v>
@@ -5703,7 +5688,7 @@
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B346" s="0" t="s">
         <v>23</v>
@@ -5714,7 +5699,7 @@
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B347" s="0" t="s">
         <v>3</v>
@@ -5725,7 +5710,7 @@
     </row>
     <row r="348" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B348" s="0" t="s">
         <v>3</v>
@@ -5736,17 +5721,17 @@
     </row>
     <row r="350" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B352" s="0" t="s">
         <v>3</v>
@@ -5757,7 +5742,7 @@
     </row>
     <row r="353" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B353" s="0" t="s">
         <v>23</v>
@@ -5768,7 +5753,7 @@
     </row>
     <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B354" s="0" t="s">
         <v>23</v>
@@ -5779,7 +5764,7 @@
     </row>
     <row r="355" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B355" s="0" t="s">
         <v>3</v>
@@ -5790,7 +5775,7 @@
     </row>
     <row r="356" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B356" s="0" t="s">
         <v>3</v>
@@ -5801,23 +5786,23 @@
     </row>
     <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B360" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C360" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D360" s="0" t="s">
         <v>5</v>
@@ -5825,21 +5810,21 @@
     </row>
     <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B361" s="0" t="s">
         <v>3</v>
       </c>
       <c r="C361" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D361" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B362" s="0" t="s">
         <v>23</v>
@@ -5850,24 +5835,24 @@
     </row>
     <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B363" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C363" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B364" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C364" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D364" s="0" t="s">
         <v>5</v>
@@ -5875,22 +5860,22 @@
     </row>
     <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B369" s="0" t="s">
         <v>3</v>
@@ -5911,7 +5896,7 @@
     </row>
     <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B373" s="0" t="s">
         <v>3</v>
@@ -5925,7 +5910,7 @@
     </row>
     <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B374" s="0" t="s">
         <v>3</v>
@@ -5941,7 +5926,7 @@
     </row>
     <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B376" s="0" t="s">
         <v>3</v>
@@ -5952,7 +5937,7 @@
     </row>
     <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B377" s="0" t="s">
         <v>3</v>
@@ -5961,28 +5946,28 @@
         <v>19</v>
       </c>
       <c r="E377" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B380" s="0" t="s">
         <v>3</v>
       </c>
       <c r="C380" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B381" s="0" t="s">
         <v>3</v>
@@ -5993,7 +5978,7 @@
     </row>
     <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B382" s="0" t="s">
         <v>3</v>
@@ -6004,7 +5989,7 @@
     </row>
     <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B383" s="0" t="s">
         <v>3</v>
@@ -6015,7 +6000,7 @@
     </row>
     <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B384" s="0" t="s">
         <v>3</v>
@@ -6026,18 +6011,18 @@
     </row>
     <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B385" s="0" t="s">
         <v>3</v>
       </c>
       <c r="C385" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B386" s="0" t="s">
         <v>3</v>
@@ -6048,7 +6033,7 @@
     </row>
     <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B387" s="0" t="s">
         <v>3</v>
@@ -6069,7 +6054,7 @@
     </row>
     <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B391" s="0" t="s">
         <v>3</v>
@@ -6080,7 +6065,7 @@
     </row>
     <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B392" s="0" t="s">
         <v>3</v>
@@ -6091,7 +6076,7 @@
     </row>
     <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B393" s="0" t="s">
         <v>3</v>
@@ -6102,7 +6087,7 @@
     </row>
     <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B394" s="0" t="s">
         <v>3</v>
@@ -6113,7 +6098,7 @@
     </row>
     <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B395" s="0" t="s">
         <v>3</v>
@@ -6129,7 +6114,7 @@
     </row>
     <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B397" s="0" t="s">
         <v>3</v>
@@ -6140,7 +6125,7 @@
     </row>
     <row r="398" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B398" s="0" t="s">
         <v>3</v>
@@ -6151,7 +6136,7 @@
     </row>
     <row r="399" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B399" s="0" t="s">
         <v>3</v>
@@ -6167,7 +6152,7 @@
     </row>
     <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B401" s="0" t="s">
         <v>3</v>
@@ -6178,7 +6163,7 @@
     </row>
     <row r="402" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B402" s="0" t="s">
         <v>3</v>
@@ -6189,7 +6174,7 @@
     </row>
     <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B403" s="0" t="s">
         <v>3</v>
@@ -6200,7 +6185,7 @@
     </row>
     <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B404" s="0" t="s">
         <v>3</v>
@@ -6211,7 +6196,7 @@
     </row>
     <row r="405" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B405" s="0" t="s">
         <v>3</v>
@@ -6222,7 +6207,7 @@
     </row>
     <row r="406" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B406" s="0" t="s">
         <v>3</v>
@@ -6233,7 +6218,7 @@
     </row>
     <row r="407" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B407" s="0" t="s">
         <v>3</v>
@@ -6244,7 +6229,7 @@
     </row>
     <row r="408" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B408" s="0" t="s">
         <v>3</v>
@@ -6255,7 +6240,7 @@
     </row>
     <row r="409" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B409" s="0" t="s">
         <v>3</v>
@@ -6276,7 +6261,7 @@
     </row>
     <row r="413" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B413" s="0" t="s">
         <v>3</v>
@@ -6287,7 +6272,7 @@
     </row>
     <row r="414" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B414" s="0" t="s">
         <v>3</v>
@@ -6298,7 +6283,7 @@
     </row>
     <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B415" s="0" t="s">
         <v>3</v>
@@ -6309,7 +6294,7 @@
     </row>
     <row r="416" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B416" s="0" t="s">
         <v>3</v>
@@ -6320,7 +6305,7 @@
     </row>
     <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B417" s="0" t="s">
         <v>3</v>
@@ -6336,7 +6321,7 @@
     </row>
     <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B419" s="0" t="s">
         <v>3</v>
@@ -6347,7 +6332,7 @@
     </row>
     <row r="420" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B420" s="0" t="s">
         <v>3</v>
@@ -6358,7 +6343,7 @@
     </row>
     <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B421" s="0" t="s">
         <v>3</v>
@@ -6369,7 +6354,7 @@
     </row>
     <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B422" s="0" t="s">
         <v>3</v>
@@ -6380,7 +6365,7 @@
     </row>
     <row r="423" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B423" s="0" t="s">
         <v>3</v>
@@ -6391,7 +6376,7 @@
     </row>
     <row r="424" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B424" s="0" t="s">
         <v>3</v>
@@ -6407,7 +6392,7 @@
     </row>
     <row r="426" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B426" s="0" t="s">
         <v>3</v>
@@ -6418,7 +6403,7 @@
     </row>
     <row r="427" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B427" s="0" t="s">
         <v>3</v>
@@ -6429,7 +6414,7 @@
     </row>
     <row r="428" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B428" s="0" t="s">
         <v>3</v>
@@ -6440,7 +6425,7 @@
     </row>
     <row r="429" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B429" s="0" t="s">
         <v>3</v>
@@ -6451,7 +6436,7 @@
     </row>
     <row r="430" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B430" s="0" t="s">
         <v>3</v>
@@ -6462,7 +6447,7 @@
     </row>
     <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B431" s="0" t="s">
         <v>3</v>
@@ -6473,7 +6458,7 @@
     </row>
     <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B432" s="0" t="s">
         <v>3</v>
@@ -6484,7 +6469,7 @@
     </row>
     <row r="433" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B433" s="0" t="s">
         <v>3</v>
@@ -6495,7 +6480,7 @@
     </row>
     <row r="434" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B434" s="0" t="s">
         <v>3</v>
@@ -6516,7 +6501,7 @@
     </row>
     <row r="438" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B438" s="0" t="s">
         <v>3</v>
@@ -6527,7 +6512,7 @@
     </row>
     <row r="439" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B439" s="0" t="s">
         <v>3</v>
@@ -6538,7 +6523,7 @@
     </row>
     <row r="440" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B440" s="0" t="s">
         <v>3</v>
@@ -6549,7 +6534,7 @@
     </row>
     <row r="441" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B441" s="0" t="s">
         <v>3</v>
@@ -6560,7 +6545,7 @@
     </row>
     <row r="442" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B442" s="0" t="s">
         <v>3</v>
@@ -6576,7 +6561,7 @@
     </row>
     <row r="444" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B444" s="0" t="s">
         <v>3</v>
@@ -6587,7 +6572,7 @@
     </row>
     <row r="445" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B445" s="0" t="s">
         <v>3</v>
@@ -6598,7 +6583,7 @@
     </row>
     <row r="446" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B446" s="0" t="s">
         <v>3</v>
@@ -6614,7 +6599,7 @@
     </row>
     <row r="448" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B448" s="0" t="s">
         <v>3</v>
@@ -6625,7 +6610,7 @@
     </row>
     <row r="449" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B449" s="0" t="s">
         <v>3</v>
@@ -6636,7 +6621,7 @@
     </row>
     <row r="450" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B450" s="0" t="s">
         <v>3</v>
@@ -6647,7 +6632,7 @@
     </row>
     <row r="451" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B451" s="0" t="s">
         <v>3</v>
@@ -6658,7 +6643,7 @@
     </row>
     <row r="452" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B452" s="0" t="s">
         <v>3</v>
@@ -6669,7 +6654,7 @@
     </row>
     <row r="453" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B453" s="0" t="s">
         <v>3</v>
@@ -6680,7 +6665,7 @@
     </row>
     <row r="454" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B454" s="0" t="s">
         <v>3</v>
@@ -6691,7 +6676,7 @@
     </row>
     <row r="455" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B455" s="0" t="s">
         <v>3</v>
@@ -6702,7 +6687,7 @@
     </row>
     <row r="456" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B456" s="0" t="s">
         <v>3</v>
@@ -6723,7 +6708,7 @@
     </row>
     <row r="460" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B460" s="0" t="s">
         <v>3</v>
@@ -6734,7 +6719,7 @@
     </row>
     <row r="461" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B461" s="0" t="s">
         <v>3</v>
@@ -6745,7 +6730,7 @@
     </row>
     <row r="462" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B462" s="0" t="s">
         <v>3</v>
@@ -6756,7 +6741,7 @@
     </row>
     <row r="463" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B463" s="0" t="s">
         <v>3</v>
@@ -6767,7 +6752,7 @@
     </row>
     <row r="464" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B464" s="0" t="s">
         <v>3</v>
@@ -6783,7 +6768,7 @@
     </row>
     <row r="466" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B466" s="0" t="s">
         <v>3</v>
@@ -6794,7 +6779,7 @@
     </row>
     <row r="467" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B467" s="0" t="s">
         <v>3</v>
@@ -6805,7 +6790,7 @@
     </row>
     <row r="468" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B468" s="0" t="s">
         <v>3</v>
@@ -6821,7 +6806,7 @@
     </row>
     <row r="470" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B470" s="0" t="s">
         <v>3</v>
@@ -6832,7 +6817,7 @@
     </row>
     <row r="471" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B471" s="0" t="s">
         <v>3</v>
@@ -6843,7 +6828,7 @@
     </row>
     <row r="472" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B472" s="0" t="s">
         <v>3</v>
@@ -6854,7 +6839,7 @@
     </row>
     <row r="473" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B473" s="0" t="s">
         <v>3</v>
@@ -6865,7 +6850,7 @@
     </row>
     <row r="474" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B474" s="0" t="s">
         <v>3</v>
@@ -6876,7 +6861,7 @@
     </row>
     <row r="475" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B475" s="0" t="s">
         <v>3</v>
@@ -6887,7 +6872,7 @@
     </row>
     <row r="476" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B476" s="0" t="s">
         <v>3</v>
@@ -6898,7 +6883,7 @@
     </row>
     <row r="477" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B477" s="0" t="s">
         <v>3</v>
@@ -6909,7 +6894,7 @@
     </row>
     <row r="478" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B478" s="0" t="s">
         <v>3</v>
@@ -6920,7 +6905,7 @@
     </row>
     <row r="480" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6930,7 +6915,7 @@
     </row>
     <row r="482" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A482" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B482" s="0" t="s">
         <v>3</v>
@@ -6941,7 +6926,7 @@
     </row>
     <row r="483" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B483" s="0" t="s">
         <v>3</v>
@@ -6952,7 +6937,7 @@
     </row>
     <row r="484" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B484" s="0" t="s">
         <v>3</v>
@@ -6963,7 +6948,7 @@
     </row>
     <row r="485" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B485" s="0" t="s">
         <v>3</v>
@@ -6974,7 +6959,7 @@
     </row>
     <row r="486" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B486" s="0" t="s">
         <v>3</v>
@@ -6985,12 +6970,12 @@
     </row>
     <row r="487" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B488" s="0" t="s">
         <v>3</v>
@@ -7001,7 +6986,7 @@
     </row>
     <row r="489" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B489" s="0" t="s">
         <v>3</v>
@@ -7012,7 +6997,7 @@
     </row>
     <row r="490" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B490" s="0" t="s">
         <v>3</v>
@@ -7023,12 +7008,12 @@
     </row>
     <row r="491" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B492" s="0" t="s">
         <v>3</v>
@@ -7039,7 +7024,7 @@
     </row>
     <row r="493" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B493" s="0" t="s">
         <v>3</v>
@@ -7050,7 +7035,7 @@
     </row>
     <row r="494" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B494" s="0" t="s">
         <v>3</v>
@@ -7066,7 +7051,7 @@
     </row>
     <row r="496" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B496" s="0" t="s">
         <v>3</v>
@@ -7077,7 +7062,7 @@
     </row>
     <row r="497" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="0" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B497" s="0" t="s">
         <v>3</v>
@@ -7088,7 +7073,7 @@
     </row>
     <row r="498" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B498" s="0" t="s">
         <v>3</v>
@@ -7099,7 +7084,7 @@
     </row>
     <row r="499" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B499" s="0" t="s">
         <v>3</v>
@@ -7110,7 +7095,7 @@
     </row>
     <row r="500" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B500" s="0" t="s">
         <v>3</v>
@@ -7121,7 +7106,7 @@
     </row>
     <row r="501" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B501" s="0" t="s">
         <v>3</v>
@@ -7137,7 +7122,7 @@
     </row>
     <row r="503" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B503" s="0" t="s">
         <v>3</v>
@@ -7148,7 +7133,7 @@
     </row>
     <row r="504" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B504" s="0" t="s">
         <v>3</v>
@@ -7159,7 +7144,7 @@
     </row>
     <row r="505" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B505" s="0" t="s">
         <v>3</v>
@@ -7170,7 +7155,7 @@
     </row>
     <row r="506" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="0" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B506" s="0" t="s">
         <v>3</v>
@@ -7181,7 +7166,7 @@
     </row>
     <row r="507" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B507" s="0" t="s">
         <v>3</v>
@@ -7192,7 +7177,7 @@
     </row>
     <row r="508" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B508" s="0" t="s">
         <v>3</v>
@@ -7203,7 +7188,7 @@
     </row>
     <row r="509" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B509" s="0" t="s">
         <v>3</v>
@@ -7214,7 +7199,7 @@
     </row>
     <row r="510" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="0" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B510" s="0" t="s">
         <v>3</v>
@@ -7225,7 +7210,7 @@
     </row>
     <row r="511" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="0" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B511" s="0" t="s">
         <v>3</v>
@@ -7246,7 +7231,7 @@
     </row>
     <row r="515" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A515" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B515" s="0" t="s">
         <v>3</v>
@@ -7257,7 +7242,7 @@
     </row>
     <row r="516" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A516" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B516" s="0" t="s">
         <v>3</v>
@@ -7271,7 +7256,7 @@
     </row>
     <row r="517" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A517" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B517" s="0" t="s">
         <v>3</v>
@@ -7282,7 +7267,7 @@
     </row>
     <row r="518" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A518" s="0" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B518" s="0" t="s">
         <v>3</v>
@@ -7296,7 +7281,7 @@
     </row>
     <row r="519" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A519" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B519" s="0" t="s">
         <v>3</v>
@@ -7307,7 +7292,7 @@
     </row>
     <row r="520" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="0" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B520" s="0" t="s">
         <v>3</v>
@@ -7318,7 +7303,7 @@
     </row>
     <row r="521" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A521" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B521" s="0" t="s">
         <v>3</v>
@@ -7329,7 +7314,7 @@
     </row>
     <row r="522" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A522" s="0" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B522" s="0" t="s">
         <v>3</v>
@@ -7340,7 +7325,7 @@
     </row>
     <row r="523" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A523" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B523" s="0" t="s">
         <v>3</v>
@@ -7351,7 +7336,7 @@
     </row>
     <row r="524" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A524" s="0" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B524" s="0" t="s">
         <v>3</v>
@@ -7362,7 +7347,7 @@
     </row>
     <row r="525" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A525" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B525" s="0" t="s">
         <v>3</v>
@@ -7373,7 +7358,7 @@
     </row>
     <row r="526" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A526" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B526" s="0" t="s">
         <v>3</v>
@@ -7387,7 +7372,7 @@
     </row>
     <row r="527" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A527" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B527" s="0" t="s">
         <v>3</v>
@@ -7398,7 +7383,7 @@
     </row>
     <row r="528" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A528" s="0" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B528" s="0" t="s">
         <v>3</v>
@@ -7412,7 +7397,7 @@
     </row>
     <row r="529" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A529" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B529" s="0" t="s">
         <v>3</v>
@@ -7423,7 +7408,7 @@
     </row>
     <row r="530" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B530" s="0" t="s">
         <v>3</v>
@@ -7434,7 +7419,7 @@
     </row>
     <row r="531" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B531" s="0" t="s">
         <v>3</v>
@@ -7445,7 +7430,7 @@
     </row>
     <row r="532" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="0" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B532" s="0" t="s">
         <v>3</v>
@@ -7456,7 +7441,7 @@
     </row>
     <row r="533" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B533" s="0" t="s">
         <v>3</v>
@@ -7467,7 +7452,7 @@
     </row>
     <row r="534" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="0" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B534" s="0" t="s">
         <v>3</v>
@@ -7483,7 +7468,7 @@
     </row>
     <row r="536" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B536" s="0" t="s">
         <v>3</v>
@@ -7494,18 +7479,18 @@
     </row>
     <row r="537" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B537" s="0" t="s">
         <v>3</v>
       </c>
       <c r="C537" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A538" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B538" s="0" t="s">
         <v>3</v>
@@ -7516,7 +7501,7 @@
     </row>
     <row r="539" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A539" s="0" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B539" s="0" t="s">
         <v>3</v>
@@ -7530,7 +7515,7 @@
     </row>
     <row r="540" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A540" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B540" s="0" t="s">
         <v>3</v>
@@ -7541,7 +7526,7 @@
     </row>
     <row r="541" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B541" s="0" t="s">
         <v>3</v>
@@ -7555,7 +7540,7 @@
     </row>
     <row r="542" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B542" s="0" t="s">
         <v>3</v>
@@ -7566,7 +7551,7 @@
     </row>
     <row r="543" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="0" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B543" s="0" t="s">
         <v>3</v>
@@ -7577,7 +7562,7 @@
     </row>
     <row r="544" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A544" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B544" s="0" t="s">
         <v>3</v>
@@ -7588,7 +7573,7 @@
     </row>
     <row r="545" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A545" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B545" s="0" t="s">
         <v>3</v>
@@ -7599,7 +7584,7 @@
     </row>
     <row r="546" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A546" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B546" s="0" t="s">
         <v>3</v>
@@ -7610,7 +7595,7 @@
     </row>
     <row r="547" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A547" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B547" s="0" t="s">
         <v>3</v>
@@ -7621,7 +7606,7 @@
     </row>
     <row r="548" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A548" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B548" s="0" t="s">
         <v>3</v>
@@ -7632,7 +7617,7 @@
     </row>
     <row r="549" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A549" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B549" s="0" t="s">
         <v>3</v>
@@ -7646,7 +7631,7 @@
     </row>
     <row r="550" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A550" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B550" s="0" t="s">
         <v>3</v>
@@ -7657,7 +7642,7 @@
     </row>
     <row r="551" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B551" s="0" t="s">
         <v>3</v>
@@ -7671,7 +7656,7 @@
     </row>
     <row r="552" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A552" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B552" s="0" t="s">
         <v>3</v>
@@ -7682,7 +7667,7 @@
     </row>
     <row r="553" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A553" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B553" s="0" t="s">
         <v>3</v>
@@ -7693,7 +7678,7 @@
     </row>
     <row r="554" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A554" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B554" s="0" t="s">
         <v>3</v>
@@ -7704,7 +7689,7 @@
     </row>
     <row r="555" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A555" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B555" s="0" t="s">
         <v>3</v>
@@ -7715,7 +7700,7 @@
     </row>
     <row r="556" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A556" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B556" s="0" t="s">
         <v>3</v>
@@ -7726,7 +7711,7 @@
     </row>
     <row r="557" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A557" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B557" s="0" t="s">
         <v>3</v>
@@ -7747,7 +7732,7 @@
     </row>
     <row r="561" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A561" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B561" s="0" t="s">
         <v>164</v>
@@ -7758,7 +7743,7 @@
     </row>
     <row r="562" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A562" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B562" s="0" t="s">
         <v>164</v>
@@ -7769,7 +7754,7 @@
     </row>
     <row r="563" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A563" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B563" s="0" t="s">
         <v>164</v>
@@ -7780,7 +7765,7 @@
     </row>
     <row r="564" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A564" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B564" s="0" t="s">
         <v>164</v>
@@ -7791,16 +7776,16 @@
     </row>
     <row r="565" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A565" s="0" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B565" s="0" t="s">
         <v>164</v>
       </c>
       <c r="C565" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E565" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="567" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7815,7 +7800,7 @@
     </row>
     <row r="569" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A569" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B569" s="0" t="s">
         <v>164</v>
@@ -7826,7 +7811,7 @@
     </row>
     <row r="570" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A570" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B570" s="0" t="s">
         <v>164</v>
@@ -7837,7 +7822,7 @@
     </row>
     <row r="571" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A571" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B571" s="0" t="s">
         <v>164</v>
@@ -7848,7 +7833,7 @@
     </row>
     <row r="572" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A572" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B572" s="0" t="s">
         <v>164</v>
@@ -7859,7 +7844,7 @@
     </row>
     <row r="573" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A573" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B573" s="0" t="s">
         <v>164</v>
@@ -7870,7 +7855,7 @@
     </row>
     <row r="574" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A574" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B574" s="0" t="s">
         <v>164</v>
@@ -7881,7 +7866,7 @@
     </row>
     <row r="575" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A575" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B575" s="0" t="s">
         <v>164</v>
@@ -7892,7 +7877,7 @@
     </row>
     <row r="576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A576" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B576" s="0" t="s">
         <v>164</v>
@@ -7903,12 +7888,12 @@
     </row>
     <row r="577" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A577" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="578" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A578" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B578" s="0" t="s">
         <v>164</v>
@@ -7919,7 +7904,7 @@
     </row>
     <row r="579" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A579" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B579" s="0" t="s">
         <v>164</v>
@@ -7930,7 +7915,7 @@
     </row>
     <row r="580" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A580" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B580" s="0" t="s">
         <v>164</v>
@@ -7941,7 +7926,7 @@
     </row>
     <row r="581" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A581" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B581" s="0" t="s">
         <v>164</v>
@@ -7952,7 +7937,7 @@
     </row>
     <row r="582" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A582" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B582" s="0" t="s">
         <v>164</v>
@@ -7963,7 +7948,7 @@
     </row>
     <row r="583" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A583" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B583" s="0" t="s">
         <v>164</v>
@@ -7974,7 +7959,7 @@
     </row>
     <row r="584" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A584" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B584" s="0" t="s">
         <v>164</v>
@@ -7985,7 +7970,7 @@
     </row>
     <row r="585" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A585" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B585" s="0" t="s">
         <v>164</v>
@@ -8001,7 +7986,7 @@
     </row>
     <row r="587" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A587" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B587" s="0" t="s">
         <v>164</v>
@@ -8012,7 +7997,7 @@
     </row>
     <row r="588" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A588" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B588" s="0" t="s">
         <v>164</v>
@@ -8023,7 +8008,7 @@
     </row>
     <row r="589" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B589" s="0" t="s">
         <v>164</v>
@@ -8034,7 +8019,7 @@
     </row>
     <row r="590" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A590" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B590" s="0" t="s">
         <v>164</v>
@@ -8045,7 +8030,7 @@
     </row>
     <row r="591" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A591" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B591" s="0" t="s">
         <v>164</v>
@@ -8056,7 +8041,7 @@
     </row>
     <row r="592" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A592" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B592" s="0" t="s">
         <v>164</v>
@@ -8067,12 +8052,12 @@
     </row>
     <row r="593" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A593" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="594" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A594" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B594" s="0" t="s">
         <v>164</v>
@@ -8083,7 +8068,7 @@
     </row>
     <row r="595" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A595" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B595" s="0" t="s">
         <v>164</v>
@@ -8094,7 +8079,7 @@
     </row>
     <row r="596" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A596" s="0" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B596" s="0" t="s">
         <v>164</v>
@@ -8105,7 +8090,7 @@
     </row>
     <row r="597" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A597" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B597" s="0" t="s">
         <v>164</v>
@@ -8116,7 +8101,7 @@
     </row>
     <row r="598" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A598" s="0" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B598" s="0" t="s">
         <v>164</v>
@@ -8127,12 +8112,12 @@
     </row>
     <row r="599" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A599" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="600" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A600" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B600" s="0" t="s">
         <v>164</v>
@@ -8143,7 +8128,7 @@
     </row>
     <row r="601" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A601" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="602" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8153,7 +8138,7 @@
     </row>
     <row r="603" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A603" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B603" s="0" t="s">
         <v>164</v>
@@ -8164,7 +8149,7 @@
     </row>
     <row r="604" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A604" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B604" s="0" t="s">
         <v>164</v>
@@ -8175,7 +8160,7 @@
     </row>
     <row r="605" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A605" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B605" s="0" t="s">
         <v>164</v>
@@ -8186,7 +8171,7 @@
     </row>
     <row r="606" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A606" s="0" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B606" s="0" t="s">
         <v>164</v>
@@ -8197,7 +8182,7 @@
     </row>
     <row r="607" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A607" s="0" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B607" s="0" t="s">
         <v>164</v>
@@ -8208,7 +8193,7 @@
     </row>
     <row r="608" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A608" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B608" s="0" t="s">
         <v>164</v>
@@ -8224,7 +8209,7 @@
     </row>
     <row r="610" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A610" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B610" s="0" t="s">
         <v>164</v>
@@ -8235,7 +8220,7 @@
     </row>
     <row r="611" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A611" s="0" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B611" s="0" t="s">
         <v>164</v>
@@ -8246,7 +8231,7 @@
     </row>
     <row r="612" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A612" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B612" s="0" t="s">
         <v>164</v>
@@ -8262,7 +8247,7 @@
     </row>
     <row r="614" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A614" s="0" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B614" s="0" t="s">
         <v>164</v>
@@ -8273,7 +8258,7 @@
     </row>
     <row r="615" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A615" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B615" s="0" t="s">
         <v>164</v>
@@ -8284,7 +8269,7 @@
     </row>
     <row r="616" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A616" s="0" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B616" s="0" t="s">
         <v>164</v>
@@ -8295,7 +8280,7 @@
     </row>
     <row r="617" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A617" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B617" s="0" t="s">
         <v>164</v>
@@ -8306,7 +8291,7 @@
     </row>
     <row r="618" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A618" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B618" s="0" t="s">
         <v>164</v>
@@ -8317,7 +8302,7 @@
     </row>
     <row r="619" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A619" s="0" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B619" s="0" t="s">
         <v>164</v>
@@ -8328,7 +8313,7 @@
     </row>
     <row r="620" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A620" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B620" s="0" t="s">
         <v>164</v>
@@ -8339,7 +8324,7 @@
     </row>
     <row r="621" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A621" s="0" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B621" s="0" t="s">
         <v>164</v>
@@ -8350,7 +8335,7 @@
     </row>
     <row r="622" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A622" s="0" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B622" s="0" t="s">
         <v>164</v>
@@ -8361,12 +8346,12 @@
     </row>
     <row r="623" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A623" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="624" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A624" s="0" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B624" s="0" t="s">
         <v>164</v>
@@ -8377,7 +8362,7 @@
     </row>
     <row r="625" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A625" s="0" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B625" s="0" t="s">
         <v>164</v>
@@ -8388,7 +8373,7 @@
     </row>
     <row r="626" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A626" s="0" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B626" s="0" t="s">
         <v>164</v>
@@ -8399,7 +8384,7 @@
     </row>
     <row r="627" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A627" s="0" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B627" s="0" t="s">
         <v>164</v>
@@ -8410,7 +8395,7 @@
     </row>
     <row r="628" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A628" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="629" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8420,7 +8405,7 @@
     </row>
     <row r="630" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A630" s="0" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B630" s="0" t="s">
         <v>164</v>
@@ -8431,7 +8416,7 @@
     </row>
     <row r="631" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A631" s="0" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B631" s="0" t="s">
         <v>164</v>
@@ -8442,7 +8427,7 @@
     </row>
     <row r="632" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A632" s="0" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B632" s="0" t="s">
         <v>164</v>
@@ -8453,7 +8438,7 @@
     </row>
     <row r="633" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A633" s="0" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B633" s="0" t="s">
         <v>164</v>
@@ -8464,7 +8449,7 @@
     </row>
     <row r="634" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A634" s="0" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B634" s="0" t="s">
         <v>164</v>
@@ -8475,7 +8460,7 @@
     </row>
     <row r="635" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A635" s="0" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B635" s="0" t="s">
         <v>164</v>
@@ -8491,7 +8476,7 @@
     </row>
     <row r="637" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A637" s="0" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B637" s="0" t="s">
         <v>164</v>
@@ -8502,7 +8487,7 @@
     </row>
     <row r="638" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A638" s="0" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B638" s="0" t="s">
         <v>164</v>
@@ -8513,7 +8498,7 @@
     </row>
     <row r="639" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A639" s="0" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B639" s="0" t="s">
         <v>164</v>
@@ -8529,7 +8514,7 @@
     </row>
     <row r="641" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A641" s="0" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B641" s="0" t="s">
         <v>164</v>
@@ -8540,7 +8525,7 @@
     </row>
     <row r="642" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A642" s="0" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B642" s="0" t="s">
         <v>164</v>
@@ -8551,7 +8536,7 @@
     </row>
     <row r="643" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A643" s="0" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B643" s="0" t="s">
         <v>164</v>
@@ -8562,7 +8547,7 @@
     </row>
     <row r="644" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A644" s="0" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B644" s="0" t="s">
         <v>164</v>
@@ -8573,7 +8558,7 @@
     </row>
     <row r="645" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A645" s="0" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B645" s="0" t="s">
         <v>164</v>
@@ -8584,7 +8569,7 @@
     </row>
     <row r="646" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="0" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B646" s="0" t="s">
         <v>164</v>
@@ -8595,7 +8580,7 @@
     </row>
     <row r="647" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="0" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B647" s="0" t="s">
         <v>164</v>
@@ -8606,7 +8591,7 @@
     </row>
     <row r="648" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A648" s="0" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B648" s="0" t="s">
         <v>164</v>
@@ -8617,7 +8602,7 @@
     </row>
     <row r="649" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="0" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B649" s="0" t="s">
         <v>164</v>
@@ -8628,7 +8613,7 @@
     </row>
     <row r="650" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="651" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8638,7 +8623,7 @@
     </row>
     <row r="652" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A652" s="0" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B652" s="0" t="s">
         <v>164</v>
@@ -8649,7 +8634,7 @@
     </row>
     <row r="653" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A653" s="0" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B653" s="0" t="s">
         <v>164</v>
@@ -8660,7 +8645,7 @@
     </row>
     <row r="654" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A654" s="0" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B654" s="0" t="s">
         <v>164</v>
@@ -8671,7 +8656,7 @@
     </row>
     <row r="655" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A655" s="0" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B655" s="0" t="s">
         <v>164</v>
@@ -8682,7 +8667,7 @@
     </row>
     <row r="656" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A656" s="0" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B656" s="0" t="s">
         <v>164</v>
@@ -8698,7 +8683,7 @@
     </row>
     <row r="658" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A658" s="0" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B658" s="0" t="s">
         <v>164</v>
@@ -8709,7 +8694,7 @@
     </row>
     <row r="659" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A659" s="0" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B659" s="0" t="s">
         <v>164</v>
@@ -8720,7 +8705,7 @@
     </row>
     <row r="660" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A660" s="0" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B660" s="0" t="s">
         <v>164</v>
@@ -8736,7 +8721,7 @@
     </row>
     <row r="662" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A662" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B662" s="0" t="s">
         <v>164</v>
@@ -8747,7 +8732,7 @@
     </row>
     <row r="663" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A663" s="0" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B663" s="0" t="s">
         <v>164</v>
@@ -8758,7 +8743,7 @@
     </row>
     <row r="664" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A664" s="0" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B664" s="0" t="s">
         <v>164</v>
@@ -8769,7 +8754,7 @@
     </row>
     <row r="665" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A665" s="0" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B665" s="0" t="s">
         <v>164</v>
@@ -8780,7 +8765,7 @@
     </row>
     <row r="666" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A666" s="0" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B666" s="0" t="s">
         <v>164</v>
@@ -8791,7 +8776,7 @@
     </row>
     <row r="667" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A667" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B667" s="0" t="s">
         <v>164</v>
@@ -8802,7 +8787,7 @@
     </row>
     <row r="668" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A668" s="0" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B668" s="0" t="s">
         <v>164</v>
@@ -8813,7 +8798,7 @@
     </row>
     <row r="669" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A669" s="0" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B669" s="0" t="s">
         <v>164</v>
@@ -8824,7 +8809,7 @@
     </row>
     <row r="670" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="0" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B670" s="0" t="s">
         <v>164</v>
@@ -8835,12 +8820,12 @@
     </row>
     <row r="671" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="672" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A672" s="0" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B672" s="0" t="s">
         <v>164</v>
@@ -8851,17 +8836,17 @@
     </row>
     <row r="674" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A674" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="675" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A675" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="676" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A676" s="0" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B676" s="0" t="s">
         <v>164</v>
@@ -8872,7 +8857,7 @@
     </row>
     <row r="677" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A677" s="0" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B677" s="0" t="s">
         <v>164</v>
@@ -8883,17 +8868,17 @@
     </row>
     <row r="679" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A679" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="680" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A680" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="681" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A681" s="0" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B681" s="0" t="s">
         <v>164</v>
@@ -8904,7 +8889,7 @@
     </row>
     <row r="682" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A682" s="0" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B682" s="0" t="s">
         <v>164</v>
@@ -8915,7 +8900,7 @@
     </row>
     <row r="683" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A683" s="0" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B683" s="0" t="s">
         <v>164</v>
@@ -8926,23 +8911,23 @@
     </row>
     <row r="685" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A685" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="686" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A686" s="0" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B686" s="0" t="s">
         <v>164</v>
       </c>
       <c r="C686" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="687" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A687" s="0" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B687" s="0" t="s">
         <v>164</v>
@@ -8953,7 +8938,7 @@
     </row>
     <row r="688" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A688" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B688" s="0" t="s">
         <v>164</v>
@@ -8964,34 +8949,34 @@
     </row>
     <row r="689" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A689" s="0" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B689" s="0" t="s">
         <v>164</v>
       </c>
       <c r="C689" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="690" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A690" s="0" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B690" s="0" t="s">
         <v>164</v>
       </c>
       <c r="C690" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="692" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A692" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="693" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A693" s="0" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B693" s="0" t="s">
         <v>164</v>
@@ -9000,12 +8985,12 @@
         <v>19</v>
       </c>
       <c r="E693" s="0" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="694" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A694" s="0" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B694" s="0" t="s">
         <v>164</v>
@@ -9014,12 +8999,12 @@
         <v>19</v>
       </c>
       <c r="E694" s="0" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="695" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A695" s="0" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B695" s="0" t="s">
         <v>164</v>
@@ -9028,12 +9013,12 @@
         <v>19</v>
       </c>
       <c r="E695" s="0" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="696" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A696" s="0" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B696" s="0" t="s">
         <v>164</v>
@@ -9042,17 +9027,17 @@
         <v>19</v>
       </c>
       <c r="E696" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="697" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A697" s="0" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="698" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A698" s="0" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B698" s="0" t="s">
         <v>164</v>
@@ -9061,12 +9046,12 @@
         <v>19</v>
       </c>
       <c r="E698" s="0" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="699" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A699" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B699" s="0" t="s">
         <v>164</v>
@@ -9075,12 +9060,12 @@
         <v>19</v>
       </c>
       <c r="E699" s="0" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="700" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A700" s="0" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B700" s="0" t="s">
         <v>164</v>
@@ -9089,12 +9074,12 @@
         <v>19</v>
       </c>
       <c r="E700" s="0" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="701" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A701" s="0" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="B701" s="0" t="s">
         <v>164</v>
@@ -9103,12 +9088,12 @@
         <v>19</v>
       </c>
       <c r="E701" s="0" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="702" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A702" s="0" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B702" s="0" t="s">
         <v>164</v>
@@ -9117,12 +9102,12 @@
         <v>19</v>
       </c>
       <c r="E702" s="0" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="703" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A703" s="0" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B703" s="0" t="s">
         <v>164</v>
@@ -9131,12 +9116,12 @@
         <v>19</v>
       </c>
       <c r="E703" s="0" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="704" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A704" s="0" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B704" s="0" t="s">
         <v>164</v>
@@ -9145,12 +9130,12 @@
         <v>19</v>
       </c>
       <c r="E704" s="0" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="705" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A705" s="0" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B705" s="0" t="s">
         <v>164</v>
@@ -9159,12 +9144,12 @@
         <v>19</v>
       </c>
       <c r="E705" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="706" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A706" s="0" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B706" s="0" t="s">
         <v>164</v>
@@ -9173,12 +9158,12 @@
         <v>19</v>
       </c>
       <c r="E706" s="0" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="707" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A707" s="0" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B707" s="0" t="s">
         <v>164</v>
@@ -9187,12 +9172,12 @@
         <v>19</v>
       </c>
       <c r="E707" s="0" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="708" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A708" s="0" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B708" s="0" t="s">
         <v>164</v>
@@ -9201,12 +9186,12 @@
         <v>19</v>
       </c>
       <c r="E708" s="0" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="709" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A709" s="0" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B709" s="0" t="s">
         <v>164</v>
@@ -9215,17 +9200,17 @@
         <v>19</v>
       </c>
       <c r="E709" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="710" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A710" s="0" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="711" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A711" s="0" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B711" s="0" t="s">
         <v>164</v>
@@ -9234,12 +9219,12 @@
         <v>19</v>
       </c>
       <c r="E711" s="0" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="712" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A712" s="0" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B712" s="0" t="s">
         <v>164</v>
@@ -9248,12 +9233,12 @@
         <v>19</v>
       </c>
       <c r="E712" s="0" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="713" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A713" s="0" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B713" s="0" t="s">
         <v>164</v>
@@ -9262,12 +9247,12 @@
         <v>19</v>
       </c>
       <c r="E713" s="0" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="714" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A714" s="0" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B714" s="0" t="s">
         <v>164</v>
@@ -9276,12 +9261,12 @@
         <v>19</v>
       </c>
       <c r="E714" s="0" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="715" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A715" s="0" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B715" s="0" t="s">
         <v>164</v>
@@ -9290,12 +9275,12 @@
         <v>19</v>
       </c>
       <c r="E715" s="0" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="716" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A716" s="0" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B716" s="0" t="s">
         <v>164</v>
@@ -9304,12 +9289,12 @@
         <v>19</v>
       </c>
       <c r="E716" s="0" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="717" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A717" s="0" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B717" s="0" t="s">
         <v>164</v>
@@ -9318,12 +9303,12 @@
         <v>19</v>
       </c>
       <c r="E717" s="0" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="718" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A718" s="0" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B718" s="0" t="s">
         <v>164</v>
@@ -9332,12 +9317,12 @@
         <v>19</v>
       </c>
       <c r="E718" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="719" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A719" s="0" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B719" s="0" t="s">
         <v>164</v>
@@ -9346,12 +9331,12 @@
         <v>19</v>
       </c>
       <c r="E719" s="0" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="720" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A720" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B720" s="0" t="s">
         <v>164</v>
@@ -9360,12 +9345,12 @@
         <v>19</v>
       </c>
       <c r="E720" s="0" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="721" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A721" s="0" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B721" s="0" t="s">
         <v>164</v>
@@ -9374,12 +9359,12 @@
         <v>19</v>
       </c>
       <c r="E721" s="0" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="722" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A722" s="0" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B722" s="0" t="s">
         <v>164</v>
@@ -9388,17 +9373,17 @@
         <v>19</v>
       </c>
       <c r="E722" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="723" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A723" s="0" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="724" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A724" s="0" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B724" s="0" t="s">
         <v>164</v>
@@ -9407,12 +9392,12 @@
         <v>19</v>
       </c>
       <c r="E724" s="0" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="725" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A725" s="0" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B725" s="0" t="s">
         <v>164</v>
@@ -9421,12 +9406,12 @@
         <v>19</v>
       </c>
       <c r="E725" s="0" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="726" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A726" s="0" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B726" s="0" t="s">
         <v>164</v>
@@ -9435,12 +9420,12 @@
         <v>19</v>
       </c>
       <c r="E726" s="0" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="727" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A727" s="0" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B727" s="0" t="s">
         <v>164</v>
@@ -9449,12 +9434,12 @@
         <v>19</v>
       </c>
       <c r="E727" s="0" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="728" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A728" s="0" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B728" s="0" t="s">
         <v>164</v>
@@ -9463,12 +9448,12 @@
         <v>19</v>
       </c>
       <c r="E728" s="0" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="729" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A729" s="0" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B729" s="0" t="s">
         <v>164</v>
@@ -9477,12 +9462,12 @@
         <v>19</v>
       </c>
       <c r="E729" s="0" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="730" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A730" s="0" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B730" s="0" t="s">
         <v>164</v>
@@ -9491,12 +9476,12 @@
         <v>19</v>
       </c>
       <c r="E730" s="0" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="731" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A731" s="0" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B731" s="0" t="s">
         <v>164</v>
@@ -9505,12 +9490,12 @@
         <v>19</v>
       </c>
       <c r="E731" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="732" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A732" s="0" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B732" s="0" t="s">
         <v>164</v>
@@ -9519,12 +9504,12 @@
         <v>19</v>
       </c>
       <c r="E732" s="0" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="733" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A733" s="0" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="B733" s="0" t="s">
         <v>164</v>
@@ -9533,12 +9518,12 @@
         <v>19</v>
       </c>
       <c r="E733" s="0" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="734" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A734" s="0" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B734" s="0" t="s">
         <v>164</v>
@@ -9547,12 +9532,12 @@
         <v>19</v>
       </c>
       <c r="E734" s="0" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="735" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A735" s="0" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B735" s="0" t="s">
         <v>164</v>
@@ -9561,17 +9546,17 @@
         <v>19</v>
       </c>
       <c r="E735" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="736" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A736" s="0" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="737" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A737" s="0" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B737" s="0" t="s">
         <v>164</v>
@@ -9580,12 +9565,12 @@
         <v>19</v>
       </c>
       <c r="E737" s="0" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="738" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A738" s="0" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B738" s="0" t="s">
         <v>164</v>
@@ -9594,12 +9579,12 @@
         <v>19</v>
       </c>
       <c r="E738" s="0" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="739" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A739" s="0" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B739" s="0" t="s">
         <v>164</v>
@@ -9608,12 +9593,12 @@
         <v>19</v>
       </c>
       <c r="E739" s="0" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="740" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A740" s="0" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B740" s="0" t="s">
         <v>164</v>
@@ -9622,12 +9607,12 @@
         <v>19</v>
       </c>
       <c r="E740" s="0" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="741" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A741" s="0" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B741" s="0" t="s">
         <v>164</v>
@@ -9636,12 +9621,12 @@
         <v>19</v>
       </c>
       <c r="E741" s="0" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="742" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A742" s="0" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B742" s="0" t="s">
         <v>164</v>
@@ -9650,12 +9635,12 @@
         <v>19</v>
       </c>
       <c r="E742" s="0" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="743" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A743" s="0" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B743" s="0" t="s">
         <v>164</v>
@@ -9664,12 +9649,12 @@
         <v>19</v>
       </c>
       <c r="E743" s="0" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="744" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A744" s="0" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B744" s="0" t="s">
         <v>164</v>
@@ -9678,12 +9663,12 @@
         <v>19</v>
       </c>
       <c r="E744" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="745" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A745" s="0" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B745" s="0" t="s">
         <v>164</v>
@@ -9692,12 +9677,12 @@
         <v>19</v>
       </c>
       <c r="E745" s="0" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="746" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A746" s="0" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B746" s="0" t="s">
         <v>164</v>
@@ -9706,12 +9691,12 @@
         <v>19</v>
       </c>
       <c r="E746" s="0" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="747" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A747" s="0" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B747" s="0" t="s">
         <v>164</v>
@@ -9720,12 +9705,12 @@
         <v>19</v>
       </c>
       <c r="E747" s="0" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="748" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A748" s="0" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B748" s="0" t="s">
         <v>164</v>
@@ -9734,17 +9719,17 @@
         <v>19</v>
       </c>
       <c r="E748" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="749" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A749" s="0" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="750" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A750" s="0" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B750" s="0" t="s">
         <v>164</v>
@@ -9753,12 +9738,12 @@
         <v>19</v>
       </c>
       <c r="E750" s="0" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="751" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A751" s="0" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="B751" s="0" t="s">
         <v>164</v>
@@ -9767,12 +9752,12 @@
         <v>19</v>
       </c>
       <c r="E751" s="0" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="752" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A752" s="0" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B752" s="0" t="s">
         <v>164</v>
@@ -9781,12 +9766,12 @@
         <v>19</v>
       </c>
       <c r="E752" s="0" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="753" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A753" s="0" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B753" s="0" t="s">
         <v>164</v>
@@ -9795,12 +9780,12 @@
         <v>19</v>
       </c>
       <c r="E753" s="0" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="754" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A754" s="0" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="B754" s="0" t="s">
         <v>164</v>
@@ -9809,12 +9794,12 @@
         <v>19</v>
       </c>
       <c r="E754" s="0" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="755" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A755" s="0" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B755" s="0" t="s">
         <v>164</v>
@@ -9823,12 +9808,12 @@
         <v>19</v>
       </c>
       <c r="E755" s="0" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="756" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A756" s="0" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B756" s="0" t="s">
         <v>164</v>
@@ -9837,12 +9822,12 @@
         <v>19</v>
       </c>
       <c r="E756" s="0" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="757" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A757" s="0" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B757" s="0" t="s">
         <v>164</v>
@@ -9851,12 +9836,12 @@
         <v>19</v>
       </c>
       <c r="E757" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="758" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A758" s="0" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B758" s="0" t="s">
         <v>164</v>
@@ -9865,12 +9850,12 @@
         <v>19</v>
       </c>
       <c r="E758" s="0" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="759" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A759" s="0" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="B759" s="0" t="s">
         <v>164</v>
@@ -9879,12 +9864,12 @@
         <v>19</v>
       </c>
       <c r="E759" s="0" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="760" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A760" s="0" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B760" s="0" t="s">
         <v>164</v>
@@ -9893,12 +9878,12 @@
         <v>19</v>
       </c>
       <c r="E760" s="0" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="761" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A761" s="0" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="B761" s="0" t="s">
         <v>164</v>
@@ -9907,7 +9892,7 @@
         <v>19</v>
       </c>
       <c r="E761" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>

</xml_diff>